<commit_message>
Cleaned up Notes Section of Repo
Reorganized and Shuffled around
</commit_message>
<xml_diff>
--- a/Notes/Science/New Science/Space Science Information.xlsx
+++ b/Notes/Science/New Science/Space Science Information.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\9CS1941\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan paplaczyk\Dropbox\GAMES\KSP\Git\RP-0\Notes\Science\New Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
     <sheet name="References" sheetId="7" r:id="rId7"/>
     <sheet name="Equipment" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="413">
   <si>
     <t>AGILE</t>
   </si>
@@ -641,7 +641,637 @@
     <t>Sputnik 6 (Korabl-Sputnik 3)</t>
   </si>
   <si>
-    <t>PAGE 148</t>
+    <t>Venera 1</t>
+  </si>
+  <si>
+    <t>Venus Flyby</t>
+  </si>
+  <si>
+    <t>Explorer 9</t>
+  </si>
+  <si>
+    <t>Density of Earth's Atmosphere with inflatable sphere</t>
+  </si>
+  <si>
+    <t>Scout (Algol, Castor, Antares, Altair)</t>
+  </si>
+  <si>
+    <t>Transit 3B</t>
+  </si>
+  <si>
+    <t>Doppler Shift Measurement for global navigation</t>
+  </si>
+  <si>
+    <t>LOFTI</t>
+  </si>
+  <si>
+    <t>Launched with Transit 3B</t>
+  </si>
+  <si>
+    <t>20-in sphere to explore low-frequency radio wave propagation</t>
+  </si>
+  <si>
+    <t>Korabl-Sputnik 4</t>
+  </si>
+  <si>
+    <t>Crewed Spaceflight Testing with Biological Animals</t>
+  </si>
+  <si>
+    <t>Korabl-Sputnik 5</t>
+  </si>
+  <si>
+    <t>Explorer 10</t>
+  </si>
+  <si>
+    <t>Rudidium-vapor Magnetometer, Fluxgate Magentometers, Plasma Probe, Optical Aspect Sensor</t>
+  </si>
+  <si>
+    <t>Vostok 1</t>
+  </si>
+  <si>
+    <t>First Human in Orbit</t>
+  </si>
+  <si>
+    <t>Explorer 11</t>
+  </si>
+  <si>
+    <t>Gamma Ray Telescope (S-15), Micrometorite (Shield), Temperature (internal), Sun &amp; Earth Sensor</t>
+  </si>
+  <si>
+    <t>Detect extraterrestrial high-energy gamma rays from neutral pi mason decay, map the spatial distribution of the decay gamma rays</t>
+  </si>
+  <si>
+    <t>Discoverer 25</t>
+  </si>
+  <si>
+    <t>Geiger Tubes, Ion Density Gauges, Micrometeorites (Density Guages)</t>
+  </si>
+  <si>
+    <t>Capsule Return</t>
+  </si>
+  <si>
+    <t>Injun 1</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Cadmium sulfide detectors, Silicon P-N junction detectors, Geiger-Mueller Tube (Anton 213), Electronc Spectrometer, Photometer (Aurora-Airglow), Fluxgate Magnetometer</t>
+  </si>
+  <si>
+    <t>Discoverer 26</t>
+  </si>
+  <si>
+    <t>Silicon, Iron, Bismuth, Yttrium, Magneisum, Nickel, Lead, Uranium (exposed to space for 50 hrs)</t>
+  </si>
+  <si>
+    <t>Explorer 12</t>
+  </si>
+  <si>
+    <t>Proton Analyzer, Magnetometer, Cosmic Ray, Ion-electron Detector</t>
+  </si>
+  <si>
+    <t>Discoverer 31</t>
+  </si>
+  <si>
+    <t>LRL Electron Spectrometer, LRL X-Ray Counter, AFCRL Proton and Alpha Particle Detector, Galactic RF Detector</t>
+  </si>
+  <si>
+    <t>TRAAC</t>
+  </si>
+  <si>
+    <t>Gravity Gradient Stabilization, Particle Detectors</t>
+  </si>
+  <si>
+    <t>Test the feasibility of a spacecraft stabilization system utilizing Earth's Gravitational Field</t>
+  </si>
+  <si>
+    <t>Injun 2</t>
+  </si>
+  <si>
+    <t>Geiger-Mueller (Type 302), Geiger-Mueller (Type 213), Photometer, Magnetometers</t>
+  </si>
+  <si>
+    <t>Secor</t>
+  </si>
+  <si>
+    <t>Range Calibration Data</t>
+  </si>
+  <si>
+    <t>Surcal</t>
+  </si>
+  <si>
+    <t>Measurement of Refraction of Radio Waves in Ionosphere</t>
+  </si>
+  <si>
+    <t>Vidicon TV Camera, Gamma-ray spectrometer, Radar Altimeter, Seismometer</t>
+  </si>
+  <si>
+    <t>OSO 1</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Make scientific observations of the sun and space</t>
+  </si>
+  <si>
+    <t>Soft X-Ray Spectrometer (10-400 Solar Radiation), Gamma Ray Detector (0.510 Mev Gamma Ray Monitor), X-Ray Detector (20-100 Kev X-Ray Monitor), Ionization Chambers (1-8 X-Ray Monitor), Dust Particle Detector (Interplanetary Dust Particle),  Solar Radiation Detector (3800-4800 Solar Radiation), Hydrogen Lyman-Alpha Detector (1100-1250 Solar Radiation), Gamma Ray Detector (0.2-1.5 Mev Solar Gamma Radiation), Gamma Ray Detector (50 Kev-3Mev Solar Gamma Radiation), Neutron Detecror, Proton-Electron Detector (Lower Van Allen Particles), High-Energy Gamma Ray Detector (100-500 Mev Solar Gamma Radiation)</t>
+  </si>
+  <si>
+    <t>Ranger 3, Ranger 4</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Microwave Radiometer</t>
+  </si>
+  <si>
+    <t>Infrared Radiometer</t>
+  </si>
+  <si>
+    <t>Energetic Particle Detectors</t>
+  </si>
+  <si>
+    <t>Micrometeroid Detector</t>
+  </si>
+  <si>
+    <t>Solar Plasma Spectrometer</t>
+  </si>
+  <si>
+    <t>Mariner 2</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Microwave Radiometer, Infrared Radiometer, Flux Gate Magentometer, Energetic Particle Detectors, Micrometeroid Detector, Solar Plasma Spectrometer</t>
+  </si>
+  <si>
+    <t>Total 41</t>
+  </si>
+  <si>
+    <t>TAVE</t>
+  </si>
+  <si>
+    <t>Accelerometers</t>
+  </si>
+  <si>
+    <t>Study the vibration during launch on a Thor-Agena</t>
+  </si>
+  <si>
+    <t>Field Strength Range from 5 to 500 Gama, Accuracy +/- 5 gamma</t>
+  </si>
+  <si>
+    <t>Ion-Electron Detector</t>
+  </si>
+  <si>
+    <t>Explorer 14</t>
+  </si>
+  <si>
+    <t>Electron Energy Distribution</t>
+  </si>
+  <si>
+    <t>Electron Angular Distribution</t>
+  </si>
+  <si>
+    <t>Omnidirectional Electron-Proton Detector</t>
+  </si>
+  <si>
+    <t>Directional Electron-Proton Detector</t>
+  </si>
+  <si>
+    <t>Explorer 15</t>
+  </si>
+  <si>
+    <t>Study radiation belt from nuclear blast</t>
+  </si>
+  <si>
+    <t>Phototelevision Camera</t>
+  </si>
+  <si>
+    <t>Mars 1</t>
+  </si>
+  <si>
+    <t>Obtain high resolution photography of Martian Surface</t>
+  </si>
+  <si>
+    <t>Infrared Spectrometer</t>
+  </si>
+  <si>
+    <t>Study distribution of organic matter on Martian Surface</t>
+  </si>
+  <si>
+    <t>Ultraviolet Spectrometer</t>
+  </si>
+  <si>
+    <t>Determine presence of ozone in the Martian Atmosphere</t>
+  </si>
+  <si>
+    <t>Magnetometer</t>
+  </si>
+  <si>
+    <t>Measure interplanetary Magnetic Field and Magnetic Field of Mars</t>
+  </si>
+  <si>
+    <t>Gas Discharge &amp; Scintillation Guages</t>
+  </si>
+  <si>
+    <t>Nuclear component of primary radiation, study Martian Radation belts</t>
+  </si>
+  <si>
+    <t>Radiotelescope</t>
+  </si>
+  <si>
+    <t>Study low-frequency Galactic Radio Noise in the 150 and 1500 m bands</t>
+  </si>
+  <si>
+    <t>Ion Traps</t>
+  </si>
+  <si>
+    <t>Study distribution of positive ions in and near Martian Atmosphere</t>
+  </si>
+  <si>
+    <t>Micrometeorite Detector</t>
+  </si>
+  <si>
+    <t>Determine momentum spectrom of dust particles</t>
+  </si>
+  <si>
+    <t>Injun 3</t>
+  </si>
+  <si>
+    <t>Proton-Electron Detector</t>
+  </si>
+  <si>
+    <t>Pulse Scintillator</t>
+  </si>
+  <si>
+    <t>APL Proton Spectrometer</t>
+  </si>
+  <si>
+    <t>Rubidium-Vapor Magnetometer</t>
+  </si>
+  <si>
+    <t>Ionization Chamber</t>
+  </si>
+  <si>
+    <t>TV Subsystem</t>
+  </si>
+  <si>
+    <t>Ranger 6</t>
+  </si>
+  <si>
+    <t>Galactic Noise</t>
+  </si>
+  <si>
+    <t>Ariel 2</t>
+  </si>
+  <si>
+    <t>Measure cosmic background radiation frequency 0.75 mc to 3.0 mc</t>
+  </si>
+  <si>
+    <t>OGO 1</t>
+  </si>
+  <si>
+    <t>Solar Cosmic Ray Physics</t>
+  </si>
+  <si>
+    <t>Plasma Electrostatic Analyzer</t>
+  </si>
+  <si>
+    <t>Plasma Faraday Cup</t>
+  </si>
+  <si>
+    <t>Positron Search &amp; Gamma Ray Spectrum</t>
+  </si>
+  <si>
+    <t>Trapped Radiation Scintillation Counter</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Isotopic Abundance</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Spectra and Fluxes</t>
+  </si>
+  <si>
+    <t>Trapped Radiation Omnidirectional Counter</t>
+  </si>
+  <si>
+    <t>Trapped Radiation Electron Spectrometer</t>
+  </si>
+  <si>
+    <t>Search Coil Magnetometer</t>
+  </si>
+  <si>
+    <t>Spherical Ion and Electron Trap</t>
+  </si>
+  <si>
+    <t>Planar Ion and Electron Trap</t>
+  </si>
+  <si>
+    <t>Radio Propagation</t>
+  </si>
+  <si>
+    <t>Interplanetary Dust Particles</t>
+  </si>
+  <si>
+    <t>VLF Noise and Propagation</t>
+  </si>
+  <si>
+    <t>Geocoronel Lyman-Alpha Scattering</t>
+  </si>
+  <si>
+    <t>Gegenschein Photometry</t>
+  </si>
+  <si>
+    <t>Measure the form and time variation of solar cosmic rays up to 90 Mev</t>
+  </si>
+  <si>
+    <t>Obtain a better understanding of low energy particles - Essential to understanding Magnetic Fields distribution</t>
+  </si>
+  <si>
+    <t>Study solar plasma an influence on Earth's magnetosphere</t>
+  </si>
+  <si>
+    <t>Determine if low energy positrons are trapped temporarily or permanently in the Van Allen Belts</t>
+  </si>
+  <si>
+    <t>Study variations in intensities of energetic particles</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Telescope to analyze the charge and energy spectrum of primary cosmic radiation</t>
+  </si>
+  <si>
+    <t>Search for acceleration mechanisms which act upon cosmic rays and solar particles</t>
+  </si>
+  <si>
+    <t>Study electron populations of the outer radiation zone of Earth</t>
+  </si>
+  <si>
+    <t>Study the injection, trapping and loss mechanisms in Earth's radiation belts</t>
+  </si>
+  <si>
+    <t>ELF frequencies in Earth's radiation belts</t>
+  </si>
+  <si>
+    <t>Very accurate magnetic field measurements</t>
+  </si>
+  <si>
+    <t>Measure concnetrations and energy of low energy charged particles</t>
+  </si>
+  <si>
+    <t>Measure radio irregularities of electrons in ionosphere and exosphere</t>
+  </si>
+  <si>
+    <t>Measure positive-ion populations</t>
+  </si>
+  <si>
+    <t>Bennet RF Mass Spectrometer</t>
+  </si>
+  <si>
+    <t>Measure velocity and mass distributions of interplanetary dust</t>
+  </si>
+  <si>
+    <t>Study noise propagation in Earth's magnetosphere</t>
+  </si>
+  <si>
+    <t>Measure radio spectrum of solar radio-noise bursts</t>
+  </si>
+  <si>
+    <t>Study scattering of Lyman-Alpha UV light</t>
+  </si>
+  <si>
+    <t>Determine the location of the Gegenschein light</t>
+  </si>
+  <si>
+    <t>Fluxgate Magentometer</t>
+  </si>
+  <si>
+    <t>Mariner 4</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Telescope</t>
+  </si>
+  <si>
+    <t>Measurement of trapped radiation near Mars and interplanetary space</t>
+  </si>
+  <si>
+    <t>Cosmic Dust Detector</t>
+  </si>
+  <si>
+    <t>Measurement of dust particle momentum and mass distribution in the Earth-Moon, Mars-Deimos-Phobos and Interplanetary region</t>
+  </si>
+  <si>
+    <t>Trapped Radiation Detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Determine the energies and identity of trapped particles in the vicinity of Mars and to monitor solar cosmic ray and energetic electrons in interplanetary space. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measure the average omnidirectional flux of corpuscular radiation and the average specific flux between Earth and Mars and in the vicinity of Mars. </t>
+  </si>
+  <si>
+    <t>Plasma Probe</t>
+  </si>
+  <si>
+    <t>Measure the spectral distribution and flux density of the positively charged component of solar plasma. The instrument was designed to measure protons in 32 energy bands within a range of 30 to 10,000 ev.</t>
+  </si>
+  <si>
+    <t>Helium Magnetometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make vector field measurements of the magnetic field in the vicinity of Earth, interplanetary space, and in the vicinity of Mars. </t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make preliminary topographic reconnaissance of portions of the surface of Mars and to obtain data on Mars surface reflectivities for the design of future systems. </t>
+  </si>
+  <si>
+    <t>Radio Wave Occultation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtain improved estimates of the surface pressure, scale height, and other characteristics of the Martian atmosphere. </t>
+  </si>
+  <si>
+    <t>Electron-Proton Angular Distrubtion and Energy Spectra</t>
+  </si>
+  <si>
+    <t>Electron-Proton Directional-Omnidirectional Detectors</t>
+  </si>
+  <si>
+    <t>Magnetic Field Meaurements</t>
+  </si>
+  <si>
+    <t>The experiment consists of a series of solid-state detectors for measuring spatial and angular distribution and energy spectra of electrons and protons.</t>
+  </si>
+  <si>
+    <t>Scintillator detectors, which were originally developed for the Relay communications satellite, measure the intensity and angular distribution of protons and electrons.</t>
+  </si>
+  <si>
+    <t>A flux gate magnetometer measures the magnitude and direction of the earth's magnetic field from 6000 miles above the earth out to Explorer's apogee.</t>
+  </si>
+  <si>
+    <t>Scintillator detector measures low-energy particles by type and energy as a function of direction, time, and position. Flown on Explorers IZ, 14, and 15</t>
+  </si>
+  <si>
+    <t>Explorer 26</t>
+  </si>
+  <si>
+    <t>Scintillator detector measures low-energy particles by type and energy as a function of direction, time, and position. Flown on Explorers 12, 14, and 15</t>
+  </si>
+  <si>
+    <t>OSO 2</t>
+  </si>
+  <si>
+    <t>Zodiacal Light Photometer</t>
+  </si>
+  <si>
+    <t>Solar X-Ray Gamma Ray Detector</t>
+  </si>
+  <si>
+    <t>Low Energy Gamma Ray Detector</t>
+  </si>
+  <si>
+    <t>High Energy Cosmic Rays</t>
+  </si>
+  <si>
+    <t>UV Spectrometer</t>
+  </si>
+  <si>
+    <t>UV Telescope and White Light Cornograph</t>
+  </si>
+  <si>
+    <t>Ion Chamber</t>
+  </si>
+  <si>
+    <t>Heavy Nuclei Chamber</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Integrating Ionization Chamber</t>
+  </si>
+  <si>
+    <t>Ranger 1</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Ionizing Radiation</t>
+  </si>
+  <si>
+    <t>Geiger-Mueller Counter</t>
+  </si>
+  <si>
+    <t>Geiger-Mueller Tube</t>
+  </si>
+  <si>
+    <t>Geiger Tube (Detector C)</t>
+  </si>
+  <si>
+    <t>Shielded Geiger Tube (Detector D)</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Detector</t>
+  </si>
+  <si>
+    <t>Explorer S-46</t>
+  </si>
+  <si>
+    <t>Geiger-Mueller Counter Cosmic Ray Telescope</t>
+  </si>
+  <si>
+    <t>IMP 1</t>
+  </si>
+  <si>
+    <t>Geiger-Mueller Counter "E"</t>
+  </si>
+  <si>
+    <t>Medium Energy Range Particle Detectors</t>
+  </si>
+  <si>
+    <t>Ranger 2</t>
+  </si>
+  <si>
+    <t>Trapped Particled Radiation Instrument</t>
+  </si>
+  <si>
+    <t>Electron Detector</t>
+  </si>
+  <si>
+    <t>Hitch-Hiker</t>
+  </si>
+  <si>
+    <t>Proton Detector</t>
+  </si>
+  <si>
+    <t>Neutron Detector</t>
+  </si>
+  <si>
+    <t>Vela</t>
+  </si>
+  <si>
+    <t>Emulsion Packs</t>
+  </si>
+  <si>
+    <t>Discoverer</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Photon Detector</t>
+  </si>
+  <si>
+    <t>Solar Corpuscular Radiation Detector</t>
+  </si>
+  <si>
+    <t>Plastic Scintillator (Detector A)</t>
+  </si>
+  <si>
+    <t>CsI Scintinallator (Detector B)</t>
+  </si>
+  <si>
+    <t>Scintillation Counter</t>
+  </si>
+  <si>
+    <t>Gamma Ray Detector</t>
+  </si>
+  <si>
+    <t>D.C. Scintillator</t>
+  </si>
+  <si>
+    <t>Gamma Ray Spectrometer</t>
+  </si>
+  <si>
+    <t>Ranger 3</t>
+  </si>
+  <si>
+    <t>Cerenkov Detector</t>
+  </si>
+  <si>
+    <t>Electron Spectrometer</t>
+  </si>
+  <si>
+    <t>Discoverer 29</t>
+  </si>
+  <si>
+    <t>CdS Broom Proton (Detector A)</t>
+  </si>
+  <si>
+    <t>CdS Low Energy Particle (Detector B)</t>
+  </si>
+  <si>
+    <t>Cadmium Sulfide Detectors</t>
+  </si>
+  <si>
+    <t>Silicon P-N Junction Detectors</t>
+  </si>
+  <si>
+    <t>Telstar 1</t>
+  </si>
+  <si>
+    <t>PAGE 562</t>
   </si>
 </sst>
 </file>
@@ -695,10 +1325,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1127,15 +1757,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1623,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,11 +2272,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2604,20 +3234,537 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="2">
+        <v>22324</v>
+      </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
+      <c r="G37" s="3">
+        <v>1419</v>
+      </c>
+      <c r="I37" t="s">
+        <v>169</v>
+      </c>
+      <c r="J37" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="A38" t="s">
+        <v>204</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="2">
+        <v>22328</v>
+      </c>
+      <c r="D38" s="4">
+        <v>399</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1607</v>
+      </c>
+      <c r="F38" s="3">
+        <v>38.86</v>
+      </c>
+      <c r="G38" s="3">
+        <v>15</v>
+      </c>
+      <c r="H38" t="s">
+        <v>206</v>
+      </c>
+      <c r="I38" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="A39" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="2">
+        <v>22334</v>
+      </c>
+      <c r="D39" s="4">
+        <v>117</v>
+      </c>
+      <c r="E39" s="4">
+        <v>511</v>
+      </c>
+      <c r="F39" s="3">
+        <v>28.4</v>
+      </c>
+      <c r="G39" s="3">
+        <v>250</v>
+      </c>
+      <c r="H39" t="s">
+        <v>176</v>
+      </c>
+      <c r="I39" t="s">
+        <v>208</v>
+      </c>
+      <c r="J39" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="A40" t="s">
+        <v>209</v>
+      </c>
+      <c r="B40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="2">
+        <v>22334</v>
+      </c>
+      <c r="D40" s="4">
+        <v>117</v>
+      </c>
+      <c r="E40" s="4">
+        <v>511</v>
+      </c>
+      <c r="F40" s="3">
+        <v>28.4</v>
+      </c>
+      <c r="G40" s="3">
+        <v>57</v>
+      </c>
+      <c r="H40" t="s">
+        <v>176</v>
+      </c>
+      <c r="I40" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="2">
+        <v>22349</v>
+      </c>
+      <c r="D41" s="4">
+        <v>114</v>
+      </c>
+      <c r="E41" s="4">
+        <v>154</v>
+      </c>
+      <c r="F41" s="3">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="G41" s="3">
+        <v>10340</v>
+      </c>
+      <c r="I41" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="2">
+        <v>22365</v>
+      </c>
+      <c r="D42" s="4">
+        <v>111</v>
+      </c>
+      <c r="E42" s="4">
+        <v>150</v>
+      </c>
+      <c r="F42" s="3">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="G42" s="3">
+        <v>10352</v>
+      </c>
+      <c r="I42" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>215</v>
+      </c>
+      <c r="B43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="2">
+        <v>22365</v>
+      </c>
+      <c r="D43" s="4">
+        <v>100</v>
+      </c>
+      <c r="E43" s="4">
+        <v>145</v>
+      </c>
+      <c r="F43" s="3">
+        <v>33</v>
+      </c>
+      <c r="G43" s="3">
+        <v>78</v>
+      </c>
+      <c r="H43" t="s">
+        <v>199</v>
+      </c>
+      <c r="I43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>217</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="2">
+        <v>22383</v>
+      </c>
+      <c r="D44" s="4">
+        <v>109</v>
+      </c>
+      <c r="E44" s="4">
+        <v>188</v>
+      </c>
+      <c r="F44" s="3">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="G44" s="3">
+        <v>10418</v>
+      </c>
+      <c r="I44" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="2">
+        <v>22398</v>
+      </c>
+      <c r="D45" s="4">
+        <v>305</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1106</v>
+      </c>
+      <c r="F45" s="3">
+        <v>28.8</v>
+      </c>
+      <c r="G45" s="3">
+        <v>95</v>
+      </c>
+      <c r="H45" t="s">
+        <v>145</v>
+      </c>
+      <c r="I45" t="s">
+        <v>220</v>
+      </c>
+      <c r="J45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>222</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="2">
+        <v>22448</v>
+      </c>
+      <c r="D46" s="4">
+        <v>139</v>
+      </c>
+      <c r="E46" s="4">
+        <v>252</v>
+      </c>
+      <c r="F46" s="3">
+        <v>82.11</v>
+      </c>
+      <c r="G46" s="3">
+        <v>300</v>
+      </c>
+      <c r="H46" t="s">
+        <v>150</v>
+      </c>
+      <c r="I46" t="s">
+        <v>223</v>
+      </c>
+      <c r="J46" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>225</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="2">
+        <v>22491</v>
+      </c>
+      <c r="D47" s="4">
+        <v>548</v>
+      </c>
+      <c r="E47" s="4">
+        <v>619</v>
+      </c>
+      <c r="F47" s="3">
+        <v>67</v>
+      </c>
+      <c r="H47" t="s">
+        <v>226</v>
+      </c>
+      <c r="I47" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C48" s="2">
+        <v>22469</v>
+      </c>
+      <c r="D48" s="4">
+        <v>146</v>
+      </c>
+      <c r="E48" s="4">
+        <v>503</v>
+      </c>
+      <c r="G48" s="3">
+        <v>300</v>
+      </c>
+      <c r="I48" t="s">
+        <v>229</v>
+      </c>
+      <c r="J48" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="2">
+        <v>22509</v>
+      </c>
+      <c r="D49" s="4">
+        <v>180</v>
+      </c>
+      <c r="E49" s="4">
+        <v>47858</v>
+      </c>
+      <c r="F49" s="3">
+        <v>33</v>
+      </c>
+      <c r="G49" s="3">
+        <v>83</v>
+      </c>
+      <c r="I49" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="2">
+        <v>22541</v>
+      </c>
+      <c r="D50" s="4">
+        <v>150</v>
+      </c>
+      <c r="E50" s="4">
+        <v>260</v>
+      </c>
+      <c r="F50" s="3">
+        <v>82.7</v>
+      </c>
+      <c r="I50" t="s">
+        <v>233</v>
+      </c>
+      <c r="J50" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>234</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="2">
+        <v>22600</v>
+      </c>
+      <c r="D51" s="4">
+        <v>562</v>
+      </c>
+      <c r="E51" s="4">
+        <v>720</v>
+      </c>
+      <c r="F51" s="3">
+        <v>32.43</v>
+      </c>
+      <c r="G51" s="3">
+        <v>240</v>
+      </c>
+      <c r="I51" t="s">
+        <v>235</v>
+      </c>
+      <c r="J51" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>237</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" s="2">
+        <v>22670</v>
+      </c>
+      <c r="I52" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>239</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" s="2">
+        <v>22670</v>
+      </c>
+      <c r="I53" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>241</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="2">
+        <v>22670</v>
+      </c>
+      <c r="I54" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>248</v>
+      </c>
+      <c r="B55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="2">
+        <v>22672</v>
+      </c>
+      <c r="G55" s="3">
+        <v>727</v>
+      </c>
+      <c r="I55" t="s">
+        <v>243</v>
+      </c>
+      <c r="J55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>244</v>
+      </c>
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="2">
+        <v>22712</v>
+      </c>
+      <c r="D56">
+        <v>344</v>
+      </c>
+      <c r="E56">
+        <v>370</v>
+      </c>
+      <c r="F56" s="3">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="G56" s="3">
+        <v>458.3</v>
+      </c>
+      <c r="H56" t="s">
+        <v>245</v>
+      </c>
+      <c r="I56" t="s">
+        <v>247</v>
+      </c>
+      <c r="J56" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>255</v>
+      </c>
+      <c r="B57" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="2">
+        <v>22885</v>
+      </c>
+      <c r="G57" s="3">
+        <v>447</v>
+      </c>
+      <c r="I57" t="s">
+        <v>257</v>
+      </c>
+      <c r="J57" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2660,90 +3807,1446 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>129</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>130</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>5.96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>132</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>8.3800000000000008</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>133</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>3.18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>134</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>1.06</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>135</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>0.46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>136</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>2.3199999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>137</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>0.97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10">
+        <v>1962</v>
+      </c>
+      <c r="D10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F10" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11">
+        <v>1962</v>
+      </c>
+      <c r="D11" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12">
+        <v>1962</v>
+      </c>
+      <c r="D12" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>252</v>
+      </c>
+      <c r="B13" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13">
+        <v>1962</v>
+      </c>
+      <c r="D13" t="s">
+        <v>258</v>
+      </c>
+      <c r="F13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14">
+        <v>1962</v>
+      </c>
+      <c r="D14" t="s">
+        <v>258</v>
+      </c>
+      <c r="F14" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>254</v>
+      </c>
+      <c r="B15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15">
+        <v>1962</v>
+      </c>
+      <c r="D15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>260</v>
+      </c>
+      <c r="B16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16">
+        <v>1962</v>
+      </c>
+      <c r="F16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B17" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17">
+        <v>1962</v>
+      </c>
+      <c r="F17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C18">
+        <v>1962</v>
+      </c>
+      <c r="F18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B19" t="s">
+        <v>269</v>
+      </c>
+      <c r="C19">
+        <v>1962</v>
+      </c>
+      <c r="F19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20" t="s">
+        <v>269</v>
+      </c>
+      <c r="C20">
+        <v>1962</v>
+      </c>
+      <c r="F20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B21" t="s">
+        <v>269</v>
+      </c>
+      <c r="C21">
+        <v>1962</v>
+      </c>
+      <c r="F21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22">
+        <v>1962</v>
+      </c>
+      <c r="F22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>274</v>
+      </c>
+      <c r="B23" t="s">
+        <v>272</v>
+      </c>
+      <c r="C23">
+        <v>1962</v>
+      </c>
+      <c r="F23" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>276</v>
+      </c>
+      <c r="B24" t="s">
+        <v>272</v>
+      </c>
+      <c r="C24">
+        <v>1962</v>
+      </c>
+      <c r="F24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>278</v>
+      </c>
+      <c r="B25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25">
+        <v>1962</v>
+      </c>
+      <c r="F25" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" t="s">
+        <v>272</v>
+      </c>
+      <c r="C26">
+        <v>1962</v>
+      </c>
+      <c r="F26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" t="s">
+        <v>272</v>
+      </c>
+      <c r="C27">
+        <v>1962</v>
+      </c>
+      <c r="F27" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>284</v>
+      </c>
+      <c r="B28" t="s">
+        <v>272</v>
+      </c>
+      <c r="C28">
+        <v>1962</v>
+      </c>
+      <c r="F28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>286</v>
+      </c>
+      <c r="B29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C29">
+        <v>1962</v>
+      </c>
+      <c r="F29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B30" t="s">
+        <v>295</v>
+      </c>
+      <c r="C30">
+        <v>1964</v>
+      </c>
+      <c r="D30">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>296</v>
+      </c>
+      <c r="B31" t="s">
+        <v>297</v>
+      </c>
+      <c r="C31">
+        <v>1964</v>
+      </c>
+      <c r="F31" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>300</v>
+      </c>
+      <c r="B32" t="s">
+        <v>299</v>
+      </c>
+      <c r="C32">
+        <v>1964</v>
+      </c>
+      <c r="D32">
+        <v>9.25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>301</v>
+      </c>
+      <c r="B33" t="s">
+        <v>299</v>
+      </c>
+      <c r="C33">
+        <v>1964</v>
+      </c>
+      <c r="D33">
+        <v>5.5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B34" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34">
+        <v>1964</v>
+      </c>
+      <c r="D34">
+        <v>11.5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>303</v>
+      </c>
+      <c r="B35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C35">
+        <v>1964</v>
+      </c>
+      <c r="D35">
+        <v>7.5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>304</v>
+      </c>
+      <c r="B36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C36">
+        <v>1964</v>
+      </c>
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>305</v>
+      </c>
+      <c r="B37" t="s">
+        <v>299</v>
+      </c>
+      <c r="C37">
+        <v>1964</v>
+      </c>
+      <c r="D37">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>306</v>
+      </c>
+      <c r="B38" t="s">
+        <v>299</v>
+      </c>
+      <c r="C38">
+        <v>1964</v>
+      </c>
+      <c r="D38">
+        <v>21.5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" t="s">
+        <v>299</v>
+      </c>
+      <c r="C39">
+        <v>1964</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>308</v>
+      </c>
+      <c r="B40" t="s">
+        <v>299</v>
+      </c>
+      <c r="C40">
+        <v>1964</v>
+      </c>
+      <c r="D40">
+        <v>14.5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>309</v>
+      </c>
+      <c r="B41" t="s">
+        <v>299</v>
+      </c>
+      <c r="C41">
+        <v>1964</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>292</v>
+      </c>
+      <c r="B42" t="s">
+        <v>299</v>
+      </c>
+      <c r="C42">
+        <v>1964</v>
+      </c>
+      <c r="D42">
+        <v>16.5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>310</v>
+      </c>
+      <c r="B43" t="s">
+        <v>299</v>
+      </c>
+      <c r="C43">
+        <v>1964</v>
+      </c>
+      <c r="D43">
+        <v>4.75</v>
+      </c>
+      <c r="F43" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>311</v>
+      </c>
+      <c r="B44" t="s">
+        <v>299</v>
+      </c>
+      <c r="C44">
+        <v>1964</v>
+      </c>
+      <c r="D44">
+        <v>15.5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>312</v>
+      </c>
+      <c r="B45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C45">
+        <v>1964</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>331</v>
+      </c>
+      <c r="B46" t="s">
+        <v>299</v>
+      </c>
+      <c r="C46">
+        <v>1964</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="F46" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>313</v>
+      </c>
+      <c r="B47" t="s">
+        <v>299</v>
+      </c>
+      <c r="C47">
+        <v>1964</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>314</v>
+      </c>
+      <c r="B48" t="s">
+        <v>299</v>
+      </c>
+      <c r="C48">
+        <v>1964</v>
+      </c>
+      <c r="D48">
+        <v>5</v>
+      </c>
+      <c r="F48" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>299</v>
+      </c>
+      <c r="C49">
+        <v>1964</v>
+      </c>
+      <c r="D49">
+        <v>4.5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>315</v>
+      </c>
+      <c r="B50" t="s">
+        <v>299</v>
+      </c>
+      <c r="C50">
+        <v>1964</v>
+      </c>
+      <c r="D50">
+        <v>3.5</v>
+      </c>
+      <c r="F50" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" t="s">
+        <v>299</v>
+      </c>
+      <c r="C51">
+        <v>1964</v>
+      </c>
+      <c r="D51">
+        <v>8.25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>339</v>
+      </c>
+      <c r="B52" t="s">
+        <v>338</v>
+      </c>
+      <c r="C52">
+        <v>1964</v>
+      </c>
+      <c r="F52" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>341</v>
+      </c>
+      <c r="B53" t="s">
+        <v>338</v>
+      </c>
+      <c r="C53">
+        <v>1964</v>
+      </c>
+      <c r="F53" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>343</v>
+      </c>
+      <c r="B54" t="s">
+        <v>338</v>
+      </c>
+      <c r="C54">
+        <v>1964</v>
+      </c>
+      <c r="F54" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>293</v>
+      </c>
+      <c r="B55" t="s">
+        <v>338</v>
+      </c>
+      <c r="C55">
+        <v>1964</v>
+      </c>
+      <c r="F55" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>346</v>
+      </c>
+      <c r="B56" t="s">
+        <v>338</v>
+      </c>
+      <c r="C56">
+        <v>1964</v>
+      </c>
+      <c r="F56" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>348</v>
+      </c>
+      <c r="B57" t="s">
+        <v>338</v>
+      </c>
+      <c r="C57">
+        <v>1964</v>
+      </c>
+      <c r="F57" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>350</v>
+      </c>
+      <c r="B58" t="s">
+        <v>338</v>
+      </c>
+      <c r="C58">
+        <v>1964</v>
+      </c>
+      <c r="F58" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>352</v>
+      </c>
+      <c r="B59" t="s">
+        <v>338</v>
+      </c>
+      <c r="C59">
+        <v>1964</v>
+      </c>
+      <c r="F59" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>354</v>
+      </c>
+      <c r="B60" t="s">
+        <v>361</v>
+      </c>
+      <c r="C60">
+        <v>1964</v>
+      </c>
+      <c r="F60" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>355</v>
+      </c>
+      <c r="B61" t="s">
+        <v>361</v>
+      </c>
+      <c r="C61">
+        <v>1964</v>
+      </c>
+      <c r="F61" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>356</v>
+      </c>
+      <c r="B62" t="s">
+        <v>361</v>
+      </c>
+      <c r="C62">
+        <v>1964</v>
+      </c>
+      <c r="F62" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>263</v>
+      </c>
+      <c r="B63" t="s">
+        <v>361</v>
+      </c>
+      <c r="C63">
+        <v>1964</v>
+      </c>
+      <c r="F63" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>354</v>
+      </c>
+      <c r="B64" t="s">
+        <v>230</v>
+      </c>
+      <c r="C64">
+        <v>1961</v>
+      </c>
+      <c r="F64" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>355</v>
+      </c>
+      <c r="B65" t="s">
+        <v>230</v>
+      </c>
+      <c r="C65">
+        <v>1961</v>
+      </c>
+      <c r="F65" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>356</v>
+      </c>
+      <c r="B66" t="s">
+        <v>230</v>
+      </c>
+      <c r="C66">
+        <v>1961</v>
+      </c>
+      <c r="F66" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>263</v>
+      </c>
+      <c r="B67" t="s">
+        <v>230</v>
+      </c>
+      <c r="C67">
+        <v>1961</v>
+      </c>
+      <c r="F67" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>263</v>
+      </c>
+      <c r="B68" t="s">
+        <v>264</v>
+      </c>
+      <c r="C68">
+        <v>1962</v>
+      </c>
+      <c r="F68" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" t="s">
+        <v>269</v>
+      </c>
+      <c r="C69">
+        <v>1962</v>
+      </c>
+      <c r="F69" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>364</v>
+      </c>
+      <c r="B70" t="s">
+        <v>363</v>
+      </c>
+      <c r="C70">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>366</v>
+      </c>
+      <c r="B71" t="s">
+        <v>363</v>
+      </c>
+      <c r="C71">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>365</v>
+      </c>
+      <c r="B72" t="s">
+        <v>363</v>
+      </c>
+      <c r="C72">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>367</v>
+      </c>
+      <c r="B73" t="s">
+        <v>363</v>
+      </c>
+      <c r="C73">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>368</v>
+      </c>
+      <c r="B74" t="s">
+        <v>363</v>
+      </c>
+      <c r="C74">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>369</v>
+      </c>
+      <c r="B75" t="s">
+        <v>363</v>
+      </c>
+      <c r="C75">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>370</v>
+      </c>
+      <c r="B76" t="s">
+        <v>141</v>
+      </c>
+      <c r="E76" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>371</v>
+      </c>
+      <c r="B77" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>372</v>
+      </c>
+      <c r="B78" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>376</v>
+      </c>
+      <c r="B79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>377</v>
+      </c>
+      <c r="B80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>376</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>378</v>
+      </c>
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>379</v>
+      </c>
+      <c r="B83" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>148</v>
+      </c>
+      <c r="B84" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>380</v>
+      </c>
+      <c r="B86" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>384</v>
+      </c>
+      <c r="B87" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>382</v>
+      </c>
+      <c r="B88" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>385</v>
+      </c>
+      <c r="B89" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>387</v>
+      </c>
+      <c r="B90" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>289</v>
+      </c>
+      <c r="B91" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>388</v>
+      </c>
+      <c r="B92" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>390</v>
+      </c>
+      <c r="B93" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>391</v>
+      </c>
+      <c r="B94" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>391</v>
+      </c>
+      <c r="B95" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>393</v>
+      </c>
+      <c r="B96" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>395</v>
+      </c>
+      <c r="B97" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>396</v>
+      </c>
+      <c r="B98" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>397</v>
+      </c>
+      <c r="B99" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>398</v>
+      </c>
+      <c r="B100" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>399</v>
+      </c>
+      <c r="B101" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>263</v>
+      </c>
+      <c r="B102" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>400</v>
+      </c>
+      <c r="B103" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>289</v>
+      </c>
+      <c r="B104" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>268</v>
+      </c>
+      <c r="B105" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>290</v>
+      </c>
+      <c r="B106" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>401</v>
+      </c>
+      <c r="B107" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>402</v>
+      </c>
+      <c r="B108" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>404</v>
+      </c>
+      <c r="B109" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>267</v>
+      </c>
+      <c r="B110" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>405</v>
+      </c>
+      <c r="B111" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>407</v>
+      </c>
+      <c r="B112" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>408</v>
+      </c>
+      <c r="B113" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>409</v>
+      </c>
+      <c r="B114" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>410</v>
+      </c>
+      <c r="B115" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>289</v>
+      </c>
+      <c r="B116" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>265</v>
+      </c>
+      <c r="B117" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>266</v>
+      </c>
+      <c r="B118" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>291</v>
+      </c>
+      <c r="B119" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>